<commit_message>
Updated Data Cleaning steps
</commit_message>
<xml_diff>
--- a/data_cleaned/cleaned_print_sales.xlsx
+++ b/data_cleaned/cleaned_print_sales.xlsx
@@ -465,7 +465,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Copies Sold</t>
+          <t>Copies_Sold</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
@@ -757,7 +757,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E7" s="2" t="n">
@@ -805,7 +805,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E8" s="2" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E24" s="2" t="n">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
@@ -2247,7 +2247,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E44" s="2" t="n">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E45" s="2" t="n">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E50" s="2" t="n">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E53" s="2" t="n">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E63" s="2" t="n">
@@ -3691,7 +3691,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E68" s="2" t="n">
@@ -3883,7 +3883,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E72" s="2" t="n">
@@ -4267,7 +4267,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E80" s="2" t="n">
@@ -4557,7 +4557,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E86" s="2" t="n">
@@ -4797,7 +4797,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E91" s="2" t="n">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E93" s="2" t="n">
@@ -5183,7 +5183,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E99" s="2" t="n">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E103" s="2" t="n">
@@ -5763,7 +5763,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E111" s="2" t="n">
@@ -6147,7 +6147,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E119" s="2" t="n">
@@ -6243,7 +6243,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E121" s="2" t="n">
@@ -6291,7 +6291,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E122" s="2" t="n">
@@ -6435,7 +6435,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E125" s="2" t="n">
@@ -6531,7 +6531,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E127" s="2" t="n">
@@ -6627,7 +6627,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E129" s="2" t="n">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E132" s="2" t="n">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E137" s="2" t="n">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E139" s="2" t="n">
@@ -7495,7 +7495,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E147" s="2" t="n">
@@ -7639,7 +7639,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E150" s="2" t="n">
@@ -7881,7 +7881,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E155" s="2" t="n">
@@ -8269,7 +8269,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E163" s="2" t="n">
@@ -8317,7 +8317,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E164" s="2" t="n">
@@ -8655,7 +8655,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E171" s="2" t="n">
@@ -8895,7 +8895,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E176" s="2" t="n">
@@ -9039,7 +9039,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E179" s="2" t="n">
@@ -9137,7 +9137,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E181" s="2" t="n">
@@ -9329,7 +9329,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E185" s="2" t="n">
@@ -9911,7 +9911,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E197" s="2" t="n">
@@ -10439,7 +10439,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E208" s="2" t="n">
@@ -10679,7 +10679,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E213" s="2" t="n">
@@ -10823,7 +10823,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E216" s="2" t="n">
@@ -11015,7 +11015,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E220" s="2" t="n">
@@ -11113,7 +11113,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E222" s="2" t="n">
@@ -11163,7 +11163,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E223" s="2" t="n">
@@ -11211,7 +11211,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E224" s="2" t="n">
@@ -11451,7 +11451,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E229" s="2" t="n">
@@ -11499,7 +11499,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E230" s="2" t="n">
@@ -11835,7 +11835,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E237" s="2" t="n">
@@ -12027,7 +12027,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E241" s="2" t="n">
@@ -12511,7 +12511,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E251" s="2" t="n">
@@ -12559,7 +12559,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E252" s="2" t="n">
@@ -13183,7 +13183,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E265" s="2" t="n">
@@ -13279,7 +13279,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E267" s="2" t="n">
@@ -13423,7 +13423,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E270" s="2" t="n">
@@ -14193,7 +14193,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E286" s="2" t="n">
@@ -14769,7 +14769,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E298" s="2" t="n">
@@ -14817,7 +14817,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E299" s="2" t="n">
@@ -15299,7 +15299,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E309" s="2" t="n">
@@ -15491,7 +15491,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E313" s="2" t="n">
@@ -15779,7 +15779,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E319" s="2" t="n">
@@ -15923,7 +15923,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E322" s="2" t="n">
@@ -16595,7 +16595,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E336" s="2" t="n">
@@ -16885,7 +16885,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E342" s="2" t="n">
@@ -17029,7 +17029,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E345" s="2" t="n">
@@ -17173,7 +17173,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E348" s="2" t="n">
@@ -17413,7 +17413,7 @@
       </c>
       <c r="D353" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E353" s="2" t="n">
@@ -17605,7 +17605,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E357" s="2" t="n">
@@ -17653,7 +17653,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E358" s="2" t="n">
@@ -17797,7 +17797,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E361" s="2" t="n">
@@ -17941,7 +17941,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E364" s="2" t="n">
@@ -18325,7 +18325,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E372" s="2" t="n">
@@ -18663,7 +18663,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E379" s="2" t="n">
@@ -18711,7 +18711,7 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E380" s="2" t="n">
@@ -18761,7 +18761,7 @@
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E381" s="2" t="n">
@@ -18905,7 +18905,7 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E384" s="2" t="n">
@@ -18953,7 +18953,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E385" s="2" t="n">
@@ -19145,7 +19145,7 @@
       </c>
       <c r="D389" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E389" s="2" t="n">
@@ -19529,7 +19529,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E397" s="2" t="n">
@@ -19817,7 +19817,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E403" s="2" t="n">
@@ -19865,7 +19865,7 @@
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E404" s="2" t="n">
@@ -19915,7 +19915,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E405" s="2" t="n">
@@ -20107,7 +20107,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E409" s="2" t="n">
@@ -20157,7 +20157,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E410" s="2" t="n">
@@ -20207,7 +20207,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E411" s="2" t="n">
@@ -20255,7 +20255,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E412" s="2" t="n">
@@ -20303,7 +20303,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E413" s="2" t="n">
@@ -20497,7 +20497,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E417" s="2" t="n">
@@ -20785,7 +20785,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E423" s="2" t="n">
@@ -20833,7 +20833,7 @@
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E424" s="2" t="n">
@@ -20929,7 +20929,7 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E426" s="2" t="n">
@@ -21073,7 +21073,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E429" s="2" t="n">
@@ -21219,7 +21219,7 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E432" s="2" t="n">
@@ -21747,7 +21747,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E443" s="2" t="n">
@@ -21845,7 +21845,7 @@
       </c>
       <c r="D445" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E445" s="2" t="n">
@@ -21991,7 +21991,7 @@
       </c>
       <c r="D448" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E448" s="2" t="n">
@@ -22523,7 +22523,7 @@
       </c>
       <c r="D459" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E459" s="2" t="n">
@@ -23057,7 +23057,7 @@
       </c>
       <c r="D470" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E470" s="2" t="n">
@@ -23297,7 +23297,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E475" s="2" t="n">
@@ -23393,7 +23393,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E477" s="2" t="n">
@@ -23537,7 +23537,7 @@
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E480" s="2" t="n">
@@ -23827,7 +23827,7 @@
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E486" s="2" t="n">
@@ -23923,7 +23923,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E488" s="2" t="n">
@@ -24309,7 +24309,7 @@
       </c>
       <c r="D496" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E496" s="2" t="n">
@@ -24987,7 +24987,7 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E510" s="2" t="n">
@@ -25421,7 +25421,7 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E519" s="2" t="n">
@@ -25855,7 +25855,7 @@
       </c>
       <c r="D528" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E528" s="2" t="n">
@@ -26533,7 +26533,7 @@
       </c>
       <c r="D542" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E542" s="2" t="n">
@@ -26677,7 +26677,7 @@
       </c>
       <c r="D545" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E545" s="2" t="n">
@@ -26775,7 +26775,7 @@
       </c>
       <c r="D547" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E547" s="2" t="n">
@@ -26919,7 +26919,7 @@
       </c>
       <c r="D550" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E550" s="2" t="n">
@@ -27881,7 +27881,7 @@
       </c>
       <c r="D570" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E570" s="2" t="n">
@@ -28123,7 +28123,7 @@
       </c>
       <c r="D575" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E575" s="2" t="n">
@@ -28171,7 +28171,7 @@
       </c>
       <c r="D576" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E576" s="2" t="n">
@@ -28653,7 +28653,7 @@
       </c>
       <c r="D586" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E586" s="2" t="n">
@@ -28893,7 +28893,7 @@
       </c>
       <c r="D591" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E591" s="2" t="n">
@@ -29519,7 +29519,7 @@
       </c>
       <c r="D604" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E604" s="2" t="n">
@@ -29855,7 +29855,7 @@
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E611" s="2" t="n">
@@ -29903,7 +29903,7 @@
       </c>
       <c r="D612" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E612" s="2" t="n">
@@ -30047,7 +30047,7 @@
       </c>
       <c r="D615" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E615" s="2" t="n">
@@ -30575,7 +30575,7 @@
       </c>
       <c r="D626" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E626" s="2" t="n">
@@ -30719,7 +30719,7 @@
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E629" s="2" t="n">
@@ -30815,7 +30815,7 @@
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E631" s="2" t="n">
@@ -30863,7 +30863,7 @@
       </c>
       <c r="D632" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E632" s="2" t="n">
@@ -30959,7 +30959,7 @@
       </c>
       <c r="D634" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E634" s="2" t="n">
@@ -31199,7 +31199,7 @@
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E639" s="2" t="n">
@@ -31491,7 +31491,7 @@
       </c>
       <c r="D645" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E645" s="2" t="n">
@@ -31977,7 +31977,7 @@
       </c>
       <c r="D655" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E655" s="2" t="n">
@@ -32025,7 +32025,7 @@
       </c>
       <c r="D656" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E656" s="2" t="n">
@@ -32217,7 +32217,7 @@
       </c>
       <c r="D660" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E660" s="2" t="n">
@@ -32699,7 +32699,7 @@
       </c>
       <c r="D670" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E670" s="2" t="n">
@@ -32987,7 +32987,7 @@
       </c>
       <c r="D676" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E676" s="2" t="n">
@@ -33133,7 +33133,7 @@
       </c>
       <c r="D679" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E679" s="2" t="n">
@@ -33471,7 +33471,7 @@
       </c>
       <c r="D686" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E686" s="2" t="n">
@@ -33567,7 +33567,7 @@
       </c>
       <c r="D688" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E688" s="2" t="n">
@@ -33759,7 +33759,7 @@
       </c>
       <c r="D692" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E692" s="2" t="n">
@@ -34293,7 +34293,7 @@
       </c>
       <c r="D703" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E703" s="2" t="n">
@@ -34389,7 +34389,7 @@
       </c>
       <c r="D705" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E705" s="2" t="n">
@@ -34871,7 +34871,7 @@
       </c>
       <c r="D715" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E715" s="2" t="n">
@@ -34919,7 +34919,7 @@
       </c>
       <c r="D716" t="inlineStr">
         <is>
-          <t>Uttar-Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E716" s="2" t="n">
@@ -34967,7 +34967,7 @@
       </c>
       <c r="D717" t="inlineStr">
         <is>
-          <t>Uttar pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E717" s="2" t="n">

</xml_diff>